<commit_message>
debugging the NiceGUI + OK
</commit_message>
<xml_diff>
--- a/inputs/2025-06-26-Seibersdorf-PGIS2_dose.input.xlsx
+++ b/inputs/2025-06-26-Seibersdorf-PGIS2_dose.input.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>name</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>trimEndAfter</t>
+  </si>
+  <si>
+    <t>variogramModel</t>
   </si>
 </sst>
 </file>
@@ -985,10 +988,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1158,6 +1161,14 @@
       </c>
       <c r="B18" s="1">
         <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>